<commit_message>
More work on reports to be transferred to campus
</commit_message>
<xml_diff>
--- a/resultsWorkbook.xlsx
+++ b/resultsWorkbook.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$M$22</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -644,7 +647,672 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean RMSE of Item and User Based CF for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Different K Values</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean RMSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-F330-4228-98F1-615BDDC0F561}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$K$2:$L$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>ItemBased</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>UserBased</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>30</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>35</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>35</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>45</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>45</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>50</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.0853999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0387</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0234000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0004999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0025999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99150000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99360000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98870000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98640000000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9879</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98540000000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98870000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98960000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9859</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99070000000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98640000000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99160000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F330-4228-98F1-615BDDC0F561}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2084395424"/>
+        <c:axId val="2079641312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2084395424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>K</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> value and Type of CF</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2079641312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2079641312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RMSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2084395424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1187,6 +1855,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1220,6 +2391,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6868B345-C240-4782-A5F5-B8AA2C49903A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1527,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +2745,7 @@
     <col min="6" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1568,10 +2775,10 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
@@ -1602,10 +2809,10 @@
       <c r="I2">
         <v>0.98970000000000002</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
       <c r="M2">
@@ -1637,11 +2844,11 @@
       <c r="I3">
         <v>1.0226</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
       </c>
       <c r="M3">
         <v>1.0387</v>
@@ -1672,11 +2879,11 @@
       <c r="I4">
         <v>1.0210999999999999</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
         <v>5</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
       </c>
       <c r="M4">
         <v>1.0234000000000001</v>
@@ -1695,11 +2902,11 @@
       <c r="D5">
         <v>0.98970000000000002</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
         <v>4</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
       </c>
       <c r="M5">
         <v>1.0004999999999999</v>
@@ -1730,11 +2937,11 @@
       <c r="I6">
         <v>0.98560000000000003</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
         <v>5</v>
-      </c>
-      <c r="L6">
-        <v>15</v>
       </c>
       <c r="M6">
         <v>1.0025999999999999</v>
@@ -1765,11 +2972,11 @@
       <c r="I7">
         <v>1.0354000000000001</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
         <v>4</v>
-      </c>
-      <c r="L7">
-        <v>15</v>
       </c>
       <c r="M7">
         <v>0.99150000000000005</v>
@@ -1800,11 +3007,11 @@
       <c r="I8">
         <v>1.0474000000000001</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
         <v>5</v>
-      </c>
-      <c r="L8">
-        <v>20</v>
       </c>
       <c r="M8">
         <v>0.99360000000000004</v>
@@ -1823,11 +3030,11 @@
       <c r="D9">
         <v>0.97150000000000003</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9">
+        <v>20</v>
+      </c>
+      <c r="L9" t="s">
         <v>4</v>
-      </c>
-      <c r="L9">
-        <v>20</v>
       </c>
       <c r="M9">
         <v>0.98860000000000003</v>
@@ -1846,11 +3053,11 @@
       <c r="D10">
         <v>0.98440000000000005</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
         <v>5</v>
-      </c>
-      <c r="L10">
-        <v>25</v>
       </c>
       <c r="M10">
         <v>0.98870000000000002</v>
@@ -1869,11 +3076,11 @@
       <c r="D11">
         <v>0.98240000000000005</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
         <v>4</v>
-      </c>
-      <c r="L11">
-        <v>25</v>
       </c>
       <c r="M11">
         <v>0.98780000000000001</v>
@@ -1892,11 +3099,11 @@
       <c r="D12">
         <v>0.94040000000000001</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
         <v>5</v>
-      </c>
-      <c r="L12">
-        <v>30</v>
       </c>
       <c r="M12">
         <v>0.98640000000000005</v>
@@ -1915,11 +3122,11 @@
       <c r="D13">
         <v>0.95130000000000003</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
         <v>4</v>
-      </c>
-      <c r="L13">
-        <v>30</v>
       </c>
       <c r="M13">
         <v>0.9879</v>
@@ -1938,11 +3145,11 @@
       <c r="D14">
         <v>0.9748</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14">
+        <v>35</v>
+      </c>
+      <c r="L14" t="s">
         <v>5</v>
-      </c>
-      <c r="L14">
-        <v>35</v>
       </c>
       <c r="M14">
         <v>0.98540000000000005</v>
@@ -1961,11 +3168,11 @@
       <c r="D15">
         <v>0.98540000000000005</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15">
+        <v>35</v>
+      </c>
+      <c r="L15" t="s">
         <v>4</v>
-      </c>
-      <c r="L15">
-        <v>35</v>
       </c>
       <c r="M15">
         <v>0.98870000000000002</v>
@@ -1984,11 +3191,11 @@
       <c r="D16">
         <v>0.98109999999999997</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16">
+        <v>40</v>
+      </c>
+      <c r="L16" t="s">
         <v>5</v>
-      </c>
-      <c r="L16">
-        <v>40</v>
       </c>
       <c r="M16">
         <v>0.98550000000000004</v>
@@ -2007,11 +3214,11 @@
       <c r="D17">
         <v>0.95109999999999995</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
         <v>4</v>
-      </c>
-      <c r="L17">
-        <v>40</v>
       </c>
       <c r="M17">
         <v>0.98960000000000004</v>
@@ -2030,11 +3237,11 @@
       <c r="D18">
         <v>0.9597</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18">
+        <v>45</v>
+      </c>
+      <c r="L18" t="s">
         <v>5</v>
-      </c>
-      <c r="L18">
-        <v>45</v>
       </c>
       <c r="M18">
         <v>0.9859</v>
@@ -2053,11 +3260,11 @@
       <c r="D19">
         <v>0.9758</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19" t="s">
         <v>4</v>
-      </c>
-      <c r="L19">
-        <v>45</v>
       </c>
       <c r="M19">
         <v>0.99070000000000003</v>
@@ -2076,11 +3283,11 @@
       <c r="D20">
         <v>0.99939999999999996</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20" t="s">
         <v>5</v>
-      </c>
-      <c r="L20">
-        <v>50</v>
       </c>
       <c r="M20">
         <v>0.98640000000000005</v>
@@ -2099,17 +3306,22 @@
       <c r="D21">
         <v>0.99329999999999996</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21">
+        <v>50</v>
+      </c>
+      <c r="L21" t="s">
         <v>4</v>
-      </c>
-      <c r="L21">
-        <v>50</v>
       </c>
       <c r="M21">
         <v>0.99160000000000004</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K1:M22">
+    <sortState ref="K2:M22">
+      <sortCondition ref="K1:K22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>